<commit_message>
change in py file excution response
</commit_message>
<xml_diff>
--- a/public/backend_automation/Admin_Admin_0000/demo/data/BrandDetails.xlsx
+++ b/public/backend_automation/Admin_Admin_0000/demo/data/BrandDetails.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Sr. No</t>
   </si>
@@ -62,25 +62,10 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>[{"id":2,"operator":"Jio","mobile_number":"89898677778","phonecode":91}]</t>
+    <t>[{"id":1,"operator":"Airtel","mobile_number":"9652356895","phonecode":91}]</t>
   </si>
   <si>
     <t>Admin Admin</t>
-  </si>
-  <si>
-    <t>Facebook</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com</t>
-  </si>
-  <si>
-    <t>Whatsapp</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Snapchat</t>
   </si>
 </sst>
 </file>
@@ -422,10 +407,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F1" sqref="F1:F5"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -438,7 +423,7 @@
     <col min="6" max="6" width="15" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="85" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="88" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="8" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="13" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -492,7 +477,7 @@
         <v>91</v>
       </c>
       <c r="E2" s="2">
-        <v>89898677778</v>
+        <v>9652356895</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -510,111 +495,6 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1">
-        <v>91</v>
-      </c>
-      <c r="E3" s="2">
-        <v>89898677778</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1">
-        <v>91</v>
-      </c>
-      <c r="E4" s="2">
-        <v>89898677778</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1">
-        <v>91</v>
-      </c>
-      <c r="E5" s="2">
-        <v>89898677778</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -631,5 +511,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>